<commit_message>
Fix DONE func in userShift (Add lastMonth: only Finished when MONTH(date)= lastMonth)
</commit_message>
<xml_diff>
--- a/CheckOut_Test.xlsx
+++ b/CheckOut_Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\GitHubDesktop_MiniStore\MiniStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,14 +18,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -71,10 +67,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -298,7 +294,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -367,7 +363,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>45105.5</v>
+        <v>45106.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>